<commit_message>
Update DR# 740 USSC Javelin Printer DNA (Batch 1) 7-11-22.xlsx
</commit_message>
<xml_diff>
--- a/DR# 740 USSC Javelin Printer DNA (Batch 1) 7-11-22.xlsx
+++ b/DR# 740 USSC Javelin Printer DNA (Batch 1) 7-11-22.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBIVELOX\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBIVELOX\Documents\GitHub\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Javelin DNA  (Single Sided)
 NU22017016
 NU22017014
-NU220170219
+NU22017029
 NU22017034
 NU22017028
 </t>
@@ -1269,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>